<commit_message>
from home PC main:Branch
</commit_message>
<xml_diff>
--- a/UIARD_cert_preparation/Merge - join - sort/Merge/Merge_Data_Excel.xlsx
+++ b/UIARD_cert_preparation/Merge - join - sort/Merge/Merge_Data_Excel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +40,42 @@
   </si>
   <si>
     <t>State</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>Column11</t>
+  </si>
+  <si>
+    <t>Column12</t>
   </si>
   <si>
     <t>AP</t>
@@ -1070,15 +1106,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1087,6 +1123,45 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1111,7 +1186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1121,8 +1196,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1131,6 +1209,9 @@
       </c>
       <c r="C5" t="s">
         <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1256,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1189,12 +1270,12 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="16:16">
       <c r="P15" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>